<commit_message>
Update ICD-10 conversions_12_17-19 (2).xlsx
</commit_message>
<xml_diff>
--- a/ICD-10 conversions_12_17-19 (2).xlsx
+++ b/ICD-10 conversions_12_17-19 (2).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shutfle1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shutfle1\Documents\GitHub\Johns-Hopkins-Overuse-Project-with-Segal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="500">
   <si>
     <t>Working Number</t>
   </si>
@@ -1929,9 +1929,6 @@
 Running on server, needs lookback (04mar2020)</t>
   </si>
   <si>
-    <t>Ready for output (17mar2020)</t>
-  </si>
-  <si>
     <t>Added revenue center codes to identify ED: https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5905698/
 0450–0459, 0981</t>
   </si>
@@ -1939,25 +1936,46 @@
     <t>ready for output (18mar2020)</t>
   </si>
   <si>
-    <t>running on cms server (18mar2020)</t>
-  </si>
-  <si>
-    <t>running on cms server (18mar2020) including lookback that includes outpatient only</t>
-  </si>
-  <si>
-    <t>running without lookback--description mentions exclusion diagnosis codes, but there are only 2 exclusion cpt codes--there are likely dx code for advanced prostate cancer that could be excluded</t>
-  </si>
-  <si>
     <t>running oncms server without lookback (19mar2020)</t>
   </si>
   <si>
     <t>running on cms server (19mar2020)</t>
   </si>
   <si>
-    <t>resulted in 0 observations on 12mar run</t>
-  </si>
-  <si>
     <t>emailed jodi with questions on 19mar2020</t>
+  </si>
+  <si>
+    <t>run again: confirm lookback and ED worked</t>
+  </si>
+  <si>
+    <t>reviewed 20mar2020, no changes needed</t>
+  </si>
+  <si>
+    <t>remove lookback</t>
+  </si>
+  <si>
+    <t>fix substring on lookback, confirm correct substring for #8 as well</t>
+  </si>
+  <si>
+    <t>change to outpatient only per 20mar2020 phone call; confirm substring correct for lookback</t>
+  </si>
+  <si>
+    <t>JS considering per 20mar2020 phone meeting; holding</t>
+  </si>
+  <si>
+    <t>resulted in 0 observations on 19mar run
+resulted in 0 observations on 12mar run
+change to use rev center instead of hcpcs/procedures per 20mar2020 phone call
+search eeg in attached: https://www.cms.gov/Regulations-and-Guidance/Guidance/Transmittals/Downloads/R167CP.pdf</t>
+  </si>
+  <si>
+    <t>running on cms server (19mar2020)--problems with ed after lookback--needs to be re-run</t>
+  </si>
+  <si>
+    <t>remove diagnosis codes per 20mar2020 phone call</t>
+  </si>
+  <si>
+    <t>20mar2020 email: change to no lookback, all screening in those age 66 and older is inappropriate</t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2454,6 +2472,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -2509,7 +2533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="281">
+  <cellXfs count="286">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3115,6 +3139,15 @@
     <xf numFmtId="0" fontId="17" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3624,11 +3657,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M174"/>
+  <dimension ref="A1:N174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
@@ -3644,7 +3677,7 @@
     <col min="9" max="9" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="228" customFormat="1" ht="77.5">
+    <row r="1" spans="1:14" s="228" customFormat="1" ht="77.5">
       <c r="A1" s="229" t="s">
         <v>355</v>
       </c>
@@ -3682,7 +3715,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="55" customFormat="1" ht="83.25" customHeight="1">
+    <row r="2" spans="1:14" s="55" customFormat="1" ht="83.25" customHeight="1">
       <c r="A2" s="232">
         <v>1</v>
       </c>
@@ -3711,11 +3744,11 @@
       <c r="J2" s="55" t="s">
         <v>454</v>
       </c>
-      <c r="L2" s="55" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="50" customFormat="1" ht="84" customHeight="1">
+      <c r="K2" s="55" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="50" customFormat="1" ht="84" customHeight="1">
       <c r="A3" s="232">
         <v>2</v>
       </c>
@@ -3747,7 +3780,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="50" customFormat="1" ht="409.5">
+    <row r="4" spans="1:14" s="50" customFormat="1" ht="409.5">
       <c r="A4" s="232">
         <v>3</v>
       </c>
@@ -3779,13 +3812,16 @@
         <v>484</v>
       </c>
       <c r="L4" s="269" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="M4" s="269" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="50" customFormat="1" ht="78">
+        <v>485</v>
+      </c>
+      <c r="N4" s="281" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="50" customFormat="1" ht="78">
       <c r="A5" s="232">
         <v>4</v>
       </c>
@@ -3817,7 +3853,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="263" customFormat="1" ht="102.75" customHeight="1">
+    <row r="6" spans="1:14" s="263" customFormat="1" ht="102.75" customHeight="1">
       <c r="A6" s="262">
         <v>5</v>
       </c>
@@ -3851,11 +3887,11 @@
       <c r="K6" s="263" t="s">
         <v>463</v>
       </c>
-      <c r="L6" s="263" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="50" customFormat="1" ht="247">
+      <c r="L6" s="282" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="50" customFormat="1" ht="247">
       <c r="A7" s="232">
         <v>6</v>
       </c>
@@ -3887,10 +3923,10 @@
         <v>471</v>
       </c>
       <c r="L7" s="50" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="50" customFormat="1" ht="108.75" customHeight="1">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="50" customFormat="1" ht="108.75" customHeight="1">
       <c r="A8" s="232">
         <v>7</v>
       </c>
@@ -3921,11 +3957,11 @@
       <c r="K8" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="L8" s="50" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="50" customFormat="1" ht="104">
+      <c r="L8" s="281" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="50" customFormat="1" ht="104">
       <c r="A9" s="232">
         <v>8</v>
       </c>
@@ -3953,11 +3989,14 @@
       <c r="J9" s="50" t="s">
         <v>453</v>
       </c>
-      <c r="L9" s="50" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="50" customFormat="1" ht="91">
+      <c r="K9" s="50" t="s">
+        <v>491</v>
+      </c>
+      <c r="L9" s="281" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="50" customFormat="1" ht="91">
       <c r="A10" s="232">
         <v>9</v>
       </c>
@@ -3989,7 +4028,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="50" customFormat="1" ht="91">
+    <row r="11" spans="1:14" s="50" customFormat="1" ht="91">
       <c r="A11" s="232">
         <v>10</v>
       </c>
@@ -4018,13 +4057,13 @@
         <v>453</v>
       </c>
       <c r="K11" s="50" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="L11" s="50" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="50" customFormat="1" ht="117">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="50" customFormat="1" ht="117">
       <c r="A12" s="232">
         <v>11</v>
       </c>
@@ -4052,11 +4091,11 @@
       <c r="J12" s="50" t="s">
         <v>453</v>
       </c>
-      <c r="L12" s="50" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="50" customFormat="1" ht="91">
+      <c r="K12" s="50" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="50" customFormat="1" ht="403">
       <c r="A13" s="232">
         <v>12</v>
       </c>
@@ -4084,14 +4123,14 @@
       <c r="J13" s="50" t="s">
         <v>453</v>
       </c>
-      <c r="K13" s="50" t="s">
-        <v>493</v>
+      <c r="K13" s="283" t="s">
+        <v>496</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="50" customFormat="1" ht="97.5" customHeight="1">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="50" customFormat="1" ht="97.5" customHeight="1">
       <c r="A14" s="232">
         <v>13</v>
       </c>
@@ -4120,10 +4159,10 @@
         <v>453</v>
       </c>
       <c r="L14" s="50" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="50" customFormat="1" ht="104">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="50" customFormat="1" ht="104">
       <c r="A15" s="232">
         <v>14</v>
       </c>
@@ -4152,7 +4191,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="50" customFormat="1" ht="117">
+    <row r="16" spans="1:14" s="50" customFormat="1" ht="117">
       <c r="A16" s="232">
         <v>15</v>
       </c>
@@ -4273,8 +4312,8 @@
       <c r="J19" s="19" t="s">
         <v>453</v>
       </c>
-      <c r="L19" s="19" t="s">
-        <v>492</v>
+      <c r="L19" s="284" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="132" customHeight="1">
@@ -4300,13 +4339,16 @@
         <v>280</v>
       </c>
       <c r="I20" s="50" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="J20" t="s">
         <v>454</v>
       </c>
       <c r="K20" t="s">
-        <v>494</v>
+        <v>489</v>
+      </c>
+      <c r="L20" s="285" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="86.25" customHeight="1">

</xml_diff>

<commit_message>
UPDATES PER 20MAR2020 PHONE CALL
</commit_message>
<xml_diff>
--- a/ICD-10 conversions_12_17-19 (2).xlsx
+++ b/ICD-10 conversions_12_17-19 (2).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shutfle1\Documents\GitHub\Johns-Hopkins-Overuse-Project-with-Segal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shutfle1\Desktop\Johns-Hopkins-Overuse-Project-with-Segal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="503">
   <si>
     <t>Working Number</t>
   </si>
@@ -1893,25 +1893,12 @@
     <t>Removed inpatient per 13mar2020 phone meeting</t>
   </si>
   <si>
-    <t>JS considering per 13mar2020 phone meeting; holding</t>
-  </si>
-  <si>
     <t>remove per 13mar2020 phone meeting</t>
   </si>
   <si>
     <t>Keep 97012 only per 13mar2020 phone call
 Make outpatient only per 13mar2020 phone call
 See why there are no outpatient per 13mar2020 phone call</t>
-  </si>
-  <si>
-    <t>ready to be run again</t>
-  </si>
-  <si>
-    <t>CMS output reviewed 13mar2020, no changes needed
-Per 06mar2020 conversation/code review: modified to include G codes for stool-based; include diagnostic that started as screening based on modifiers for colonoscopy; change to 85 as age cut-off; removed diagnostic codes not generally associated with screening</t>
-  </si>
-  <si>
-    <t>on hold per 13mar2020 phone call</t>
   </si>
   <si>
     <t xml:space="preserve">71010, 71020 </t>
@@ -1960,29 +1947,152 @@
     <t>change to outpatient only per 20mar2020 phone call; confirm substring correct for lookback</t>
   </si>
   <si>
-    <t>JS considering per 20mar2020 phone meeting; holding</t>
-  </si>
-  <si>
     <t>resulted in 0 observations on 19mar run
 resulted in 0 observations on 12mar run
 change to use rev center instead of hcpcs/procedures per 20mar2020 phone call
 search eeg in attached: https://www.cms.gov/Regulations-and-Guidance/Guidance/Transmittals/Downloads/R167CP.pdf</t>
   </si>
   <si>
-    <t>running on cms server (19mar2020)--problems with ed after lookback--needs to be re-run</t>
-  </si>
-  <si>
     <t>remove diagnosis codes per 20mar2020 phone call</t>
   </si>
   <si>
-    <t>20mar2020 email: change to no lookback, all screening in those age 66 and older is inappropriate</t>
+    <r>
+      <t xml:space="preserve">CMS output reviewed 13mar2020, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no changes needed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Per 06mar2020 conversation/code review: modified to include G codes for stool-based; include diagnostic that started as screening based on modifiers for colonoscopy; change to 85 as age cut-off; removed diagnostic codes not generally associated with screening</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on hold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> per 13mar2020 phone call</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CMS output reviewed 06mar2020, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no changes needed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>20mar2020 email: change to no lookback, all screening in those age 66 and older is inappropriate--</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eliana to make changes</t>
+    </r>
+  </si>
+  <si>
+    <t>running on cms server (20mar2020)</t>
+  </si>
+  <si>
+    <t>problem with ED lookback</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reviewed 20mar2020, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no changes needed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JS considering per 20mar2020 phone meeting; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>holding</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JS considering per 13mar2020 phone meeting; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>holding</t>
+    </r>
+  </si>
+  <si>
+    <t>RUNNING (20MAR2020)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="39">
+  <fonts count="40">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2250,6 +2360,13 @@
       <i/>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3659,9 +3776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
@@ -3745,7 +3862,7 @@
         <v>454</v>
       </c>
       <c r="K2" s="55" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="50" customFormat="1" ht="84" customHeight="1">
@@ -3809,16 +3926,16 @@
         <v>453</v>
       </c>
       <c r="K4" s="269" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="L4" s="269" t="s">
+        <v>482</v>
+      </c>
+      <c r="M4" s="269" t="s">
+        <v>481</v>
+      </c>
+      <c r="N4" s="281" t="s">
         <v>486</v>
-      </c>
-      <c r="M4" s="269" t="s">
-        <v>485</v>
-      </c>
-      <c r="N4" s="281" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="50" customFormat="1" ht="78">
@@ -3888,7 +4005,7 @@
         <v>463</v>
       </c>
       <c r="L6" s="282" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="50" customFormat="1" ht="247">
@@ -3958,7 +4075,7 @@
         <v>474</v>
       </c>
       <c r="L8" s="281" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="50" customFormat="1" ht="104">
@@ -3990,10 +4107,10 @@
         <v>453</v>
       </c>
       <c r="K9" s="50" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L9" s="281" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="50" customFormat="1" ht="91">
@@ -4025,7 +4142,7 @@
         <v>453</v>
       </c>
       <c r="K10" s="50" t="s">
-        <v>475</v>
+        <v>501</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="50" customFormat="1" ht="91">
@@ -4057,10 +4174,10 @@
         <v>453</v>
       </c>
       <c r="K11" s="50" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="L11" s="50" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="50" customFormat="1" ht="117">
@@ -4092,7 +4209,7 @@
         <v>453</v>
       </c>
       <c r="K12" s="50" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="50" customFormat="1" ht="403">
@@ -4124,10 +4241,10 @@
         <v>453</v>
       </c>
       <c r="K13" s="283" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="50" customFormat="1" ht="97.5" customHeight="1">
@@ -4158,6 +4275,9 @@
       <c r="J14" s="50" t="s">
         <v>453</v>
       </c>
+      <c r="K14" s="50" t="s">
+        <v>498</v>
+      </c>
       <c r="L14" s="50" t="s">
         <v>497</v>
       </c>
@@ -4249,10 +4369,10 @@
         <v>453</v>
       </c>
       <c r="K17" s="269" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>478</v>
+        <v>497</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="50" customFormat="1" ht="156">
@@ -4312,8 +4432,11 @@
       <c r="J19" s="19" t="s">
         <v>453</v>
       </c>
-      <c r="L19" s="284" t="s">
-        <v>498</v>
+      <c r="K19" s="284" t="s">
+        <v>492</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="132" customHeight="1">
@@ -4345,10 +4468,10 @@
         <v>454</v>
       </c>
       <c r="K20" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="L20" s="285" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="86.25" customHeight="1">
@@ -4380,7 +4503,7 @@
         <v>454</v>
       </c>
       <c r="K21" t="s">
-        <v>462</v>
+        <v>495</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="409.5">
@@ -4412,7 +4535,7 @@
         <v>454</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="104">
@@ -4444,7 +4567,7 @@
         <v>453</v>
       </c>
       <c r="K23" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="210" customFormat="1">
@@ -14048,7 +14171,7 @@
         <v>117</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -14154,7 +14277,7 @@
         <v>119</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -15540,7 +15663,7 @@
         <v>466</v>
       </c>
       <c r="E117" s="210" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F117" s="210"/>
       <c r="G117" s="210"/>
@@ -15587,10 +15710,10 @@
         <v>3</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="E118" s="210" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F118" s="210"/>
       <c r="G118" s="210"/>

</xml_diff>